<commit_message>
More Info  regarding COVID
Adding more information regarding to covid on the final report
</commit_message>
<xml_diff>
--- a/Data/4_Clean data/ASEAN_HDI.xlsx
+++ b/Data/4_Clean data/ASEAN_HDI.xlsx
@@ -8,24 +8,56 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Git\World-WIde-COVID\Data\4_Clean data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D731A92D-8776-44F6-9641-72488584CBAB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DF7BEDB8-6685-4E54-B928-35597D0C9A72}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="HDI" sheetId="1" r:id="rId1"/>
+    <sheet name="additional_info" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
+<file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
+<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
+  <metadataTypes count="1">
+    <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
+  </metadataTypes>
+  <futureMetadata name="XLDAPR" count="1">
+    <bk>
+      <extLst>
+        <ext uri="{bdbb8cdc-fa1e-496e-a857-3c3f30c029c3}">
+          <xda:dynamicArrayProperties fDynamic="1" fCollapsed="0"/>
+        </ext>
+      </extLst>
+    </bk>
+  </futureMetadata>
+  <cellMetadata count="1">
+    <bk>
+      <rc t="1" v="0"/>
+    </bk>
+  </cellMetadata>
+</metadata>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="25">
   <si>
     <t>Country</t>
   </si>
@@ -61,16 +93,70 @@
   </si>
   <si>
     <t>``</t>
+  </si>
+  <si>
+    <t>Classification</t>
+  </si>
+  <si>
+    <t>point</t>
+  </si>
+  <si>
+    <t>classification</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Very high </t>
+  </si>
+  <si>
+    <t xml:space="preserve">High </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Medium </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Low </t>
+  </si>
+  <si>
+    <t>East Asia and the Pacific</t>
+  </si>
+  <si>
+    <t>Developing Country</t>
+  </si>
+  <si>
+    <t>Brunei</t>
+  </si>
+  <si>
+    <t>Laos</t>
+  </si>
+  <si>
+    <t>Additional Information</t>
+  </si>
+  <si>
+    <t>Point</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <numFmts count="2">
+    <numFmt numFmtId="164" formatCode="#,###,##0.000"/>
+    <numFmt numFmtId="166" formatCode="0.000"/>
+  </numFmts>
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -84,7 +170,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -107,13 +193,47 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -396,8 +516,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:I11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E3" sqref="E3"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="L7" sqref="L7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -724,4 +844,208 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EFFBCD60-CBB5-46BE-AA95-A0EE64FE4A93}">
+  <dimension ref="A1:G11"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="C8" sqref="C8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="29.109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.5546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="29.109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="5.6640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11.5546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="17.33203125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A1" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="D1" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="G1" s="6"/>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A2" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="B2" s="2">
+        <v>0.89600000000000002</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="E2" s="4">
+        <v>0.93899999999999995</v>
+      </c>
+      <c r="F2" s="1" t="str" cm="1">
+        <f t="array" ref="F2">IF(E2&lt;B$5,A$5,IF(E2&lt;B$3,A$4,IF(E2&lt;B$2,A$3,IF(E2&gt;B$2,A$2,error))))</f>
+        <v xml:space="preserve">Very high </v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A3" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="B3" s="2">
+        <v>0.754</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="E3" s="4">
+        <v>0.82899999999999996</v>
+      </c>
+      <c r="F3" s="1" t="str" cm="1">
+        <f t="array" ref="F3">IF(E3&lt;B$5,A$5,IF(E3&lt;B$3,A$4,IF(E3&lt;B$2,A$3,IF(E3&gt;B$2,A$2,error))))</f>
+        <v xml:space="preserve">High </v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A4" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="B4" s="2">
+        <v>0.63600000000000001</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E4" s="4">
+        <v>0.80300000000000005</v>
+      </c>
+      <c r="F4" s="1" t="str" cm="1">
+        <f t="array" ref="F4">IF(E4&lt;B$5,A$5,IF(E4&lt;B$3,A$4,IF(E4&lt;B$2,A$3,IF(E4&gt;B$2,A$2,error))))</f>
+        <v xml:space="preserve">High </v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A5" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="B5" s="2">
+        <v>0.51800000000000002</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="E5" s="4">
+        <v>0.8</v>
+      </c>
+      <c r="F5" s="1" t="str" cm="1">
+        <f t="array" ref="F5">IF(E5&lt;B$5,A$5,IF(E5&lt;B$3,A$4,IF(E5&lt;B$2,A$3,IF(E5&gt;B$2,A$2,error))))</f>
+        <v xml:space="preserve">High </v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="D6" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="E6" s="4">
+        <v>0.70499999999999996</v>
+      </c>
+      <c r="F6" s="1" t="str" cm="1">
+        <f t="array" ref="F6">IF(E6&lt;B$5,A$5,IF(E6&lt;B$3,A$4,IF(E6&lt;B$2,A$3,IF(E6&gt;B$2,A$2,error))))</f>
+        <v xml:space="preserve">Medium </v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A7" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="E7" s="4">
+        <v>0.70299999999999996</v>
+      </c>
+      <c r="F7" s="1" t="str" cm="1">
+        <f t="array" ref="F7">IF(E7&lt;B$5,A$5,IF(E7&lt;B$3,A$4,IF(E7&lt;B$2,A$3,IF(E7&gt;B$2,A$2,error))))</f>
+        <v xml:space="preserve">Medium </v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A8" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="B8" s="7">
+        <v>0.749</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E8" s="4">
+        <v>0.69899999999999995</v>
+      </c>
+      <c r="F8" s="1" t="str" cm="1">
+        <f t="array" ref="F8">IF(E8&lt;B$5,A$5,IF(E8&lt;B$3,A$4,IF(E8&lt;B$2,A$3,IF(E8&gt;B$2,A$2,error))))</f>
+        <v xml:space="preserve">Medium </v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A9" s="10" t="s">
+        <v>20</v>
+      </c>
+      <c r="B9" s="7">
+        <v>0.68500000000000005</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="E9" s="4">
+        <v>0.60699999999999998</v>
+      </c>
+      <c r="F9" s="1" t="str" cm="1">
+        <f t="array" ref="F9">IF(E9&lt;B$5,A$5,IF(E9&lt;B$3,A$4,IF(E9&lt;B$2,A$3,IF(E9&gt;B$2,A$2,error))))</f>
+        <v xml:space="preserve">Medium </v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="D10" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E10" s="4">
+        <v>0.59299999999999997</v>
+      </c>
+      <c r="F10" s="1" t="str" cm="1">
+        <f t="array" ref="F10">IF(E10&lt;B$5,A$5,IF(E10&lt;B$3,A$4,IF(E10&lt;B$2,A$3,IF(E10&gt;B$2,A$2,error))))</f>
+        <v xml:space="preserve">Medium </v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="D11" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E11" s="4">
+        <v>0.58499999999999996</v>
+      </c>
+      <c r="F11" s="1" t="str" cm="1">
+        <f t="array" ref="F11">IF(E11&lt;B$5,A$5,IF(E11&lt;B$3,A$4,IF(E11&lt;B$2,A$3,IF(E11&gt;B$2,A$2,error))))</f>
+        <v xml:space="preserve">Medium </v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>